<commit_message>
update repo with latest testset
</commit_message>
<xml_diff>
--- a/src/test/resources/data/SSCS_cases.xlsx
+++ b/src/test/resources/data/SSCS_cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanmcadam/simple-gatling-tests-framework/bulk-scan-performance-tests/src/test/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB6AC9D-705C-1A49-A0B3-58E0E447FF84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5366AC0-1201-8243-9A4D-6ED9135666A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16000" xr2:uid="{C2CBB7CE-1862-9D48-83D0-34305EAF522C}"/>
   </bookViews>
@@ -388,8 +388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39335F78-5D73-C14D-B368-FA8B56987D24}">
   <dimension ref="A1:B107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A14"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -467,282 +467,282 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>1108249</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>1108248</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="A12" s="1">
         <v>1108247</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="A13" s="1">
         <v>1108246</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="A14" s="1">
         <v>1108245</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="A15" s="1">
         <v>1108244</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="A16" s="1">
         <v>1108243</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="A17" s="1">
         <v>1108242</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18">
+      <c r="A18" s="1">
         <v>1108241</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19">
+      <c r="A19" s="1">
         <v>1108240</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20">
+      <c r="A20" s="1">
         <v>1108239</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="A21" s="1">
         <v>1108238</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22">
+      <c r="A22" s="1">
         <v>1108237</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23">
+      <c r="A23" s="1">
         <v>1108236</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24">
+      <c r="A24" s="1">
         <v>1108235</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25">
+      <c r="A25" s="1">
         <v>1108234</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26">
+      <c r="A26" s="1">
         <v>1108233</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27">
+      <c r="A27" s="1">
         <v>1108232</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28">
+      <c r="A28" s="1">
         <v>1108231</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29">
+      <c r="A29" s="1">
         <v>1108230</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30">
+      <c r="A30" s="1">
         <v>1108162</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31">
+      <c r="A31" s="1">
         <v>1108157</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32">
+      <c r="A32" s="1">
         <v>1108155</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33">
+      <c r="A33" s="1">
         <v>1108189</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34">
+      <c r="A34" s="1">
         <v>1108186</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35">
+      <c r="A35" s="1">
         <v>1108182</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36">
+      <c r="A36" s="1">
         <v>1108179</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37">
+      <c r="A37" s="1">
         <v>1108177</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38">
+      <c r="A38" s="1">
         <v>1108173</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39">
+      <c r="A39" s="1">
         <v>1108171</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40">
+      <c r="A40" s="1">
         <v>1108161</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41">
+      <c r="A41" s="1">
         <v>1108158</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42">
+      <c r="A42" s="1">
         <v>1108225</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43">
+      <c r="A43" s="1">
         <v>1108222</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44">
+      <c r="A44" s="1">
         <v>1108224</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
rebuilt body request for fully functional upload step
</commit_message>
<xml_diff>
--- a/src/test/resources/data/SSCS_cases.xlsx
+++ b/src/test/resources/data/SSCS_cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanmcadam/simple-gatling-tests-framework/bulk-scan-performance-tests/src/test/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D71B97-C3B7-1647-BB47-DB9541BEF8C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0111DB-4B9E-D149-8FDE-DFE322C7BC6B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16000" xr2:uid="{C2CBB7CE-1862-9D48-83D0-34305EAF522C}"/>
   </bookViews>
@@ -388,8 +388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39335F78-5D73-C14D-B368-FA8B56987D24}">
   <dimension ref="A1:B107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:B59"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60:B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -867,82 +867,82 @@
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60">
+      <c r="A60" s="1">
         <v>1108211</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61">
+      <c r="A61" s="1">
         <v>1108210</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62">
+      <c r="A62" s="1">
         <v>1108209</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63">
+      <c r="A63" s="1">
         <v>1108208</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64">
+      <c r="A64" s="1">
         <v>1108207</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65">
+      <c r="A65" s="1">
         <v>1108206</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66">
+      <c r="A66" s="1">
         <v>1108205</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67">
+      <c r="A67" s="1">
         <v>1108204</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68">
+      <c r="A68" s="1">
         <v>1108203</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69">
+      <c r="A69" s="1">
         <v>1108202</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>